<commit_message>
added checkout wireframe and updated excel plan
</commit_message>
<xml_diff>
--- a/Documentation/Work_layout.xlsx
+++ b/Documentation/Work_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonathynMajor\Documents\GIT\ChitChat_Coffee\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6DBD1F-DB81-49F7-A845-1B967F995AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E1B39-5728-40B7-8CDC-5131405C16C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{6E19E911-D0F3-4E5E-AAFD-276FD76CC502}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6E19E911-D0F3-4E5E-AAFD-276FD76CC502}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
   <si>
     <t>Members</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t xml:space="preserve">Create Database functionality to Ensure new items are posted immediately. </t>
+  </si>
+  <si>
+    <t>EST. SPRINT</t>
   </si>
 </sst>
 </file>
@@ -228,15 +231,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -468,11 +477,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -547,6 +593,27 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -865,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB10CD3-8862-4C66-8847-A8B5A9F82DA1}">
   <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E16"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A504B48-57BA-454D-87E4-7641E6E5E424}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,11 +1184,12 @@
     <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:10" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15"/>
       <c r="B2" s="17" t="s">
         <v>14</v>
@@ -1147,8 +1215,11 @@
       <c r="I2" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1173,11 +1244,14 @@
       <c r="H3" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="28" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="31">
+        <v>43844</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <v>2</v>
       </c>
@@ -1202,11 +1276,14 @@
       <c r="H4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="32">
+        <v>43846</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23">
         <v>3</v>
       </c>
@@ -1231,11 +1308,14 @@
       <c r="H5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="29" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J5" s="32">
+        <v>43848</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>4</v>
       </c>
@@ -1260,19 +1340,34 @@
       <c r="H6" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="32">
+        <v>43851</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23">
+        <v>5</v>
+      </c>
+      <c r="B7" s="26"/>
       <c r="C7" s="25" t="s">
         <v>54</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="32">
+        <v>43853</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
footer updates and finished Checkout page, will need to change it upon adding functionality
</commit_message>
<xml_diff>
--- a/Documentation/Work_layout.xlsx
+++ b/Documentation/Work_layout.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JonathynMajor\Documents\GIT\ChitChat_Coffee\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E1B39-5728-40B7-8CDC-5131405C16C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A118A19-EA1A-4634-B18E-4C1BA7F1D96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6E19E911-D0F3-4E5E-AAFD-276FD76CC502}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{6E19E911-D0F3-4E5E-AAFD-276FD76CC502}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprints" sheetId="2" r:id="rId2"/>
+    <sheet name="database set up" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprints" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>Members</t>
   </si>
@@ -208,13 +209,106 @@
   </si>
   <si>
     <t>EST. SPRINT</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
+  </si>
+  <si>
+    <t>inv</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>ex.png</t>
+  </si>
+  <si>
+    <t>{data}</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone number</t>
+  </si>
+  <si>
+    <t>Jimmy Tim</t>
+  </si>
+  <si>
+    <t>Jtim</t>
+  </si>
+  <si>
+    <t>padkeqvlkqeri3qr</t>
+  </si>
+  <si>
+    <t>Jimmytime@gmail.com</t>
+  </si>
+  <si>
+    <t>555-555-5555</t>
+  </si>
+  <si>
+    <t>street address</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>line2</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>userid (fk)</t>
+  </si>
+  <si>
+    <t>product id(fk)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +320,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -245,7 +347,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -514,11 +616,120 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -616,8 +827,29 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -932,7 +1164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB10CD3-8862-4C66-8847-A8B5A9F82DA1}">
   <dimension ref="B1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
@@ -1166,6 +1398,210 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E829C04-7A2C-404E-A3E6-5702D74450D4}">
+  <dimension ref="D4:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="39" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="43">
+        <v>1</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="44">
+        <v>2.95</v>
+      </c>
+      <c r="I7" s="44">
+        <v>35</v>
+      </c>
+      <c r="J7" s="45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D10" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="L10" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="M10" s="35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="43">
+        <v>1234231</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="38"/>
+    </row>
+    <row r="12" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="36">
+        <v>1</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="4:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="50">
+        <v>1</v>
+      </c>
+      <c r="E19" s="51">
+        <v>1234231</v>
+      </c>
+      <c r="F19" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="36">
+        <v>2</v>
+      </c>
+      <c r="E20" s="37">
+        <v>1234231</v>
+      </c>
+      <c r="F20" s="38">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H11" r:id="rId1" xr:uid="{7388D548-51A9-4890-BD04-C42F8A05C0ED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A504B48-57BA-454D-87E4-7641E6E5E424}">
   <dimension ref="A1:J8"/>
   <sheetViews>

</xml_diff>